<commit_message>
[COMPRAS] Adicionado coluna periodo entrega no relatório Fixado a coluna de configuração de valor por categoria
</commit_message>
<xml_diff>
--- a/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
+++ b/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">NUMERO DE REQUISIÇÃO</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">PREÇO TOTAL COM GESTÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERÍODO ENTREGA</t>
   </si>
 </sst>
 </file>
@@ -155,12 +158,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -261,214 +268,217 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:P10"/>
+  <dimension ref="B2:Q10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="20.91"/>
   </cols>
   <sheetData>
-    <row r="2" s="2" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3" t="s">
+    <row r="2" s="3" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="Q2" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[COMPRAS] - adição de colunas no relatório. Alteração da planilha modelo
</commit_message>
<xml_diff>
--- a/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
+++ b/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">NUMERO DE REQUISIÇÃO</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t xml:space="preserve">PERÍODO ENTREGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VERBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORNECEDOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATEGORIA</t>
   </si>
 </sst>
 </file>
@@ -268,10 +280,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:Q10"/>
+  <dimension ref="B2:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -292,6 +304,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="20.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="32.77"/>
   </cols>
   <sheetData>
     <row r="2" s="3" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -342,6 +358,18 @@
       </c>
       <c r="Q2" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[COMPRAS] - versão 1.3.6 Adição de colunas no relatório. Alteração da planilha modelo
(cherry picked from commit 56c1c199424342250c6d268d749769c82ceffbdf)
</commit_message>
<xml_diff>
--- a/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
+++ b/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">NUMERO DE REQUISIÇÃO</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t xml:space="preserve">PERÍODO ENTREGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VERBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORNECEDOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATEGORIA</t>
   </si>
 </sst>
 </file>
@@ -268,10 +280,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:Q10"/>
+  <dimension ref="B2:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -292,6 +304,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="20.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="32.77"/>
   </cols>
   <sheetData>
     <row r="2" s="3" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -342,6 +358,18 @@
       </c>
       <c r="Q2" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[COMPRAS] - Pacote 5 de melhorias
</commit_message>
<xml_diff>
--- a/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
+++ b/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Planilha2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t xml:space="preserve">NUMERO DE REQUISIÇÃO</t>
   </si>
@@ -70,16 +71,26 @@
     <t xml:space="preserve">PERÍODO ENTREGA</t>
   </si>
   <si>
+    <t xml:space="preserve">STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORNECEDOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATEGORIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO Nº</t>
+  </si>
+  <si>
     <t xml:space="preserve">VERBA</t>
   </si>
   <si>
-    <t xml:space="preserve">STATUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FORNECEDOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CATEGORIA</t>
+    <t xml:space="preserve">PEDIDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIFERENÇA
+ (orçado x realizado)</t>
   </si>
 </sst>
 </file>
@@ -90,7 +101,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -121,8 +132,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +152,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
         <bgColor rgb="FF000080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -170,7 +195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -201,6 +226,26 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -230,7 +275,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -280,13 +325,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:U10"/>
+  <dimension ref="B1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.11"/>
@@ -304,12 +349,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="20.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="29.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="32.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="32.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" s="3" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -368,9 +414,7 @@
       <c r="T2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="U2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6"/>
@@ -517,4 +561,62 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:G2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.76"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" s="8" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[COMPRAS] - Adicionado a coluna Usuário Requisitante
</commit_message>
<xml_diff>
--- a/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
+++ b/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t xml:space="preserve">NUMERO DE REQUISIÇÃO</t>
   </si>
@@ -91,6 +91,9 @@
   <si>
     <t xml:space="preserve">DIFERENÇA
  (orçado x realizado)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USUÁRIO  REQUISITANTE</t>
   </si>
 </sst>
 </file>
@@ -568,10 +571,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G2"/>
+  <dimension ref="B1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -580,6 +583,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="26.12"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,7 +594,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" s="8" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="8" customFormat="true" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
@@ -608,6 +612,9 @@
       </c>
       <c r="G2" s="12" t="s">
         <v>16</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[COMPRAS][FEATURES] - Relatório de Requisições adicionar coluna data solicitação
(cherry picked from commit a4b04617461d41456755a7ef8108f16d3e6cd160)
</commit_message>
<xml_diff>
--- a/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
+++ b/wca.compras.backend/wca.compras.application/Files/excel/modelo_relatorio_requisicoes.xlsx
@@ -21,9 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t xml:space="preserve">NUMERO DE REQUISIÇÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA SOLICITAÇÃO</t>
   </si>
   <si>
     <t xml:space="preserve">RESPONSÁVEL DA RC</t>
@@ -100,9 +103,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -198,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,6 +212,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -223,11 +231,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,11 +255,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,232 +352,242 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:U10"/>
+  <dimension ref="B2:V10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="11.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="13.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="13.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="20.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="29.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="32.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="3" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="20.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="32.76"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" s="3" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="s">
+    <row r="2" s="4" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="1"/>
+      <c r="U2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -571,50 +605,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H2"/>
+  <dimension ref="B1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="18.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.12"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" s="8" customFormat="true" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="12" t="s">
+    <row r="1" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" s="11" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="17" t="s">
         <v>23</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>